<commit_message>
Update data loading and add gitignore
</commit_message>
<xml_diff>
--- a/collections_data.xlsx
+++ b/collections_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RVS\Documents\Custom Office Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RVS\Documents\Automation Files\your-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3664694-3725-414C-9DE7-BCC43B009248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DA1708-DDEC-455A-AC6B-B2365822E36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E56DA7C5-2630-460B-9A28-C83E4E74D534}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -131,7 +130,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,12 +161,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -674,10 +667,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>